<commit_message>
version 1 with modification in the first cell
</commit_message>
<xml_diff>
--- a/zero.xlsx
+++ b/zero.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,21 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>bbb</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -114,7 +122,7 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -149,7 +157,7 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -331,12 +339,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>